<commit_message>
[main] review fixed document
</commit_message>
<xml_diff>
--- a/doc/Cinemax_Schedule.xlsx
+++ b/doc/Cinemax_Schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>No</t>
     <phoneticPr fontId="2"/>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>Login/SignUp</t>
+  </si>
+  <si>
+    <t>Code Paung</t>
+  </si>
+  <si>
+    <t>Group4</t>
   </si>
 </sst>
 </file>
@@ -563,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -819,7 +825,7 @@
         <v>44516</v>
       </c>
       <c r="F12" s="4">
-        <v>44519</v>
+        <v>44518</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="2"/>
@@ -841,7 +847,7 @@
         <v>44516</v>
       </c>
       <c r="F13" s="4">
-        <v>44519</v>
+        <v>44518</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -863,7 +869,7 @@
         <v>44516</v>
       </c>
       <c r="F14" s="4">
-        <v>44519</v>
+        <v>44518</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -885,7 +891,7 @@
         <v>44516</v>
       </c>
       <c r="F15" s="4">
-        <v>44519</v>
+        <v>44518</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="2"/>
@@ -897,10 +903,18 @@
       <c r="B16" s="2">
         <v>13</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="C16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="4">
+        <v>44519</v>
+      </c>
+      <c r="F16" s="4">
+        <v>44519</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>

</xml_diff>